<commit_message>
ZSS-1191 Fine tune test case
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/1191-color-filter.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/1191-color-filter.xlsx
@@ -430,67 +430,90 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A2:A12"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:1" hidden="1">
+    <row r="1" spans="1:5">
+      <c r="E1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" hidden="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" hidden="1">
+    <row r="3" spans="1:5" hidden="1">
       <c r="A3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" hidden="1">
+    <row r="4" spans="1:5" hidden="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:5">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" hidden="1">
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1">
       <c r="A6" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" hidden="1">
+    <row r="7" spans="1:5" hidden="1">
       <c r="A7" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" hidden="1">
+    <row r="8" spans="1:5" hidden="1">
       <c r="A8" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" hidden="1">
+    <row r="9" spans="1:5" hidden="1">
       <c r="A9" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" hidden="1">
+    <row r="10" spans="1:5" hidden="1">
       <c r="A10" s="9">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" hidden="1">
+    <row r="11" spans="1:5" hidden="1">
       <c r="A11" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" hidden="1">
+    <row r="12" spans="1:5" hidden="1">
       <c r="A12">
         <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="E14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="E15">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>